<commit_message>
Ajustes do banco de dados na VM
</commit_message>
<xml_diff>
--- a/Backlog/Produck backlog.xlsx
+++ b/Backlog/Produck backlog.xlsx
@@ -1,20 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28623"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28827"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Dell\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Dell\Documents\Projeto individual\Meu-projeto-individual-\Backlog\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D2924604-B6EC-4F00-8493-728CB5CBE396}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E28D6038-C0BC-499D-8772-6B1A2D450688}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" firstSheet="1" activeTab="4" xr2:uid="{AB679324-3DC8-4F8A-B107-B10CD92536BF}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{AB679324-3DC8-4F8A-B107-B10CD92536BF}"/>
   </bookViews>
   <sheets>
     <sheet name="Product Backlog" sheetId="8" r:id="rId1"/>
-    <sheet name="Product Backlog pendente" sheetId="3" r:id="rId2"/>
+    <sheet name="Product Backlog pendente" sheetId="3" state="hidden" r:id="rId2"/>
     <sheet name="Fibonacci por Sprint" sheetId="7" r:id="rId3"/>
     <sheet name="Legenda" sheetId="6" r:id="rId4"/>
     <sheet name="Sugestões para requisitos" sheetId="5" r:id="rId5"/>
@@ -992,9 +992,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A2CC2174-7EA5-46CA-8013-802EE6D154BF}">
   <dimension ref="B1:L34"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="C1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="L6" sqref="L6:L7"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A19" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B1" sqref="B1:L32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="35.1" customHeight="1" thickTop="1" thickBottom="1" x14ac:dyDescent="0.3"/>
@@ -1003,11 +1003,10 @@
     <col min="2" max="2" width="41.5703125" style="7" customWidth="1"/>
     <col min="3" max="3" width="69.28515625" style="7" customWidth="1"/>
     <col min="4" max="4" width="17.7109375" style="6" customWidth="1"/>
-    <col min="5" max="5" width="14" style="6" customWidth="1"/>
-    <col min="6" max="6" width="12.140625" style="6" customWidth="1"/>
-    <col min="7" max="7" width="14.85546875" style="6" customWidth="1"/>
+    <col min="5" max="6" width="7.7109375" style="6" customWidth="1"/>
+    <col min="7" max="7" width="14.85546875" style="6" hidden="1" customWidth="1"/>
     <col min="8" max="8" width="10.5703125" style="6" customWidth="1"/>
-    <col min="9" max="9" width="34" style="6" customWidth="1"/>
+    <col min="9" max="9" width="32.140625" style="6" customWidth="1"/>
     <col min="10" max="11" width="11.28515625" style="6" customWidth="1"/>
     <col min="12" max="12" width="11.5703125" style="6" bestFit="1" customWidth="1"/>
     <col min="13" max="16384" width="9.140625" style="1"/>
@@ -1117,7 +1116,7 @@
         <v>8</v>
       </c>
       <c r="L3" s="4" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="4" spans="2:12" ht="35.1" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -1153,7 +1152,7 @@
         <v>8</v>
       </c>
       <c r="L4" s="4" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="5" spans="2:12" ht="35.1" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -1189,7 +1188,7 @@
         <v>8</v>
       </c>
       <c r="L5" s="4" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="6" spans="2:12" ht="35.1" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -1297,7 +1296,7 @@
         <v>8</v>
       </c>
       <c r="L8" s="4" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="9" spans="2:12" ht="35.1" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -1333,7 +1332,7 @@
         <v>8</v>
       </c>
       <c r="L9" s="4" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="10" spans="2:12" ht="35.1" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -1369,7 +1368,7 @@
         <v>8</v>
       </c>
       <c r="L10" s="4" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="11" spans="2:12" ht="35.1" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -1405,7 +1404,7 @@
         <v>8</v>
       </c>
       <c r="L11" s="4" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="12" spans="2:12" ht="35.1" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -1441,7 +1440,7 @@
         <v>8</v>
       </c>
       <c r="L12" s="4" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="13" spans="2:12" ht="35.1" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -1477,7 +1476,7 @@
         <v>8</v>
       </c>
       <c r="L13" s="4" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="14" spans="2:12" ht="35.1" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -1513,7 +1512,7 @@
         <v>83</v>
       </c>
       <c r="L14" s="4" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="15" spans="2:12" ht="35.1" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -1549,7 +1548,7 @@
         <v>79</v>
       </c>
       <c r="L15" s="4" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="16" spans="2:12" ht="35.1" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -1585,7 +1584,7 @@
         <v>79</v>
       </c>
       <c r="L16" s="4" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="17" spans="2:12" ht="35.1" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -1621,7 +1620,7 @@
         <v>79</v>
       </c>
       <c r="L17" s="4" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="18" spans="2:12" ht="35.1" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -1657,7 +1656,7 @@
         <v>78</v>
       </c>
       <c r="L18" s="4" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="19" spans="2:12" ht="35.1" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -1693,7 +1692,7 @@
         <v>78</v>
       </c>
       <c r="L19" s="4" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="20" spans="2:12" ht="35.1" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -1729,7 +1728,7 @@
         <v>78</v>
       </c>
       <c r="L20" s="4" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="21" spans="2:12" ht="35.1" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -1765,7 +1764,7 @@
         <v>78</v>
       </c>
       <c r="L21" s="4" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="22" spans="2:12" ht="35.1" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -1873,7 +1872,7 @@
         <v>78</v>
       </c>
       <c r="L24" s="4" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="25" spans="2:12" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -1909,7 +1908,7 @@
         <v>78</v>
       </c>
       <c r="L25" s="4" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="26" spans="2:12" ht="35.1" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -1945,7 +1944,7 @@
         <v>84</v>
       </c>
       <c r="L26" s="4" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="27" spans="2:12" ht="35.1" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -1981,7 +1980,7 @@
         <v>86</v>
       </c>
       <c r="L27" s="4" t="s">
-        <v>63</v>
+        <v>39</v>
       </c>
     </row>
     <row r="28" spans="2:12" ht="35.1" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -2017,7 +2016,7 @@
         <v>86</v>
       </c>
       <c r="L28" s="4" t="s">
-        <v>63</v>
+        <v>39</v>
       </c>
     </row>
     <row r="29" spans="2:12" ht="35.1" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -2053,7 +2052,7 @@
         <v>86</v>
       </c>
       <c r="L29" s="4" t="s">
-        <v>63</v>
+        <v>39</v>
       </c>
     </row>
     <row r="30" spans="2:12" ht="35.1" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -2089,7 +2088,7 @@
         <v>86</v>
       </c>
       <c r="L30" s="4" t="s">
-        <v>63</v>
+        <v>39</v>
       </c>
     </row>
     <row r="31" spans="2:12" ht="35.1" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -2125,7 +2124,7 @@
         <v>86</v>
       </c>
       <c r="L31" s="4" t="s">
-        <v>63</v>
+        <v>39</v>
       </c>
     </row>
     <row r="32" spans="2:12" ht="35.1" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -2161,7 +2160,7 @@
         <v>86</v>
       </c>
       <c r="L32" s="4" t="s">
-        <v>63</v>
+        <v>39</v>
       </c>
     </row>
     <row r="34" spans="2:2" ht="35.1" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -2190,7 +2189,7 @@
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
-      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" disablePrompts="1" count="1">
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{1D3784B8-2696-4778-8EDF-A4011C7AD0C8}">
           <x14:formula1>
             <xm:f>Fibonacci!$D$7:$D$11</xm:f>
@@ -2208,7 +2207,7 @@
   <dimension ref="B1:L59"/>
   <sheetViews>
     <sheetView showGridLines="0" topLeftCell="C1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A13" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="K13" sqref="K13:K19"/>
     </sheetView>
   </sheetViews>
@@ -3213,25 +3212,25 @@
     <row r="36" ht="35.1" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="37" ht="35.1" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="38" ht="35.1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="40" ht="35.1" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="41" ht="35.1" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="42" ht="35.1" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="43" ht="35.1" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="44" ht="35.1" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="45" ht="35.1" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="46" ht="35.1" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="47" ht="35.1" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="48" ht="35.1" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="49" ht="35.1" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="51" ht="35.1" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="52" ht="35.1" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="53" ht="35.1" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="54" ht="35.1" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="40" ht="35.1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="41" ht="35.1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="42" ht="35.1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="43" ht="35.1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="44" ht="35.1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="45" ht="35.1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="46" ht="35.1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="47" ht="35.1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="48" ht="35.1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="49" ht="35.1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="51" ht="35.1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="52" ht="35.1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="53" ht="35.1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="54" ht="35.1" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="55" ht="35.1" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="56" ht="35.1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="57" ht="35.1" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="57" ht="35.1" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="58" ht="35.1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="59" ht="35.1" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="59" ht="35.1" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <autoFilter ref="B1:L27" xr:uid="{831A3FE2-A405-481B-8C5B-5096A2CC35E1}">
     <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B2:L27">
@@ -3451,7 +3450,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B56EC897-511D-459E-B2A6-5083809C3FA0}">
   <dimension ref="B1:K4"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+    <sheetView showGridLines="0" workbookViewId="0">
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>

</xml_diff>